<commit_message>
Updated V1.1 to support optional ZIF sockets
</commit_message>
<xml_diff>
--- a/6502 ROR Test Board BOM V1.1.xlsx
+++ b/6502 ROR Test Board BOM V1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony gaming rig\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC0774E-20D0-4F50-BDC0-CC5A86DD14AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD728C-7909-45AE-912C-20CED0C4F4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF81D018-8F28-45BB-9BEF-AA2F6781CE47}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Part</t>
   </si>
@@ -95,9 +95,6 @@
     <t>https://www.digikey.com/en/products/detail/mill-max-manufacturing-corp./110-44-628-41-001000/947065?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-947065_sig-Cj0KCQiAsvWrBhC0ARIsAO4E6f-n5nWNgybS2qUO86ZqxEnQ_h0rnbVowhkTPqAOPzXCz3sslOpRflsaApoTEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQiAsvWrBhC0ARIsAO4E6f-n5nWNgybS2qUO86ZqxEnQ_h0rnbVowhkTPqAOPzXCz3sslOpRflsaApoTEALw_wcB</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/CTS-Electronic-Components/MXO45-3C-1M0000?qs=hbgUSdfWRJUFs0kP0zCadA%3D%3D</t>
   </si>
   <si>
@@ -138,6 +135,36 @@
   </si>
   <si>
     <t>2N7000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 pin dip socket </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc./SA083040/3313521?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-3313521_sig-CjwKCAiAhJWsBhAaEiwAmrNyq5dclVZk8-MBYFG0oFTDynfyj3FFGwbIrs7jaRJfWEbyVEt59HuM7xoCXo8QAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAhJWsBhAaEiwAmrNyq5dclVZk8-MBYFG0oFTDynfyj3FFGwbIrs7jaRJfWEbyVEt59HuM7xoCXo8QAvD_BwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 pin dip socket </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc./SA143040/3313523?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-3313523_sig-CjwKCAiAhJWsBhAaEiwAmrNyqxTndQQCCuQQPSV_d0JFNoRku27pWZsp-P1NJmj3MW2GJU_XtduBPxoC2n8QAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAhJWsBhAaEiwAmrNyqxTndQQCCuQQPSV_d0JFNoRku27pWZsp-P1NJmj3MW2GJU_XtduBPxoC2n8QAvD_BwE</t>
+  </si>
+  <si>
+    <t>Normal Dip Sockets</t>
+  </si>
+  <si>
+    <t>ZIF Sockets</t>
+  </si>
+  <si>
+    <t>40 pin ZIF socket</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/383#description</t>
+  </si>
+  <si>
+    <t>28 pin ZIF socket</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/264998977768</t>
   </si>
 </sst>
 </file>
@@ -169,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -192,12 +219,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -212,6 +276,25 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -527,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D92E306-8B80-4CAD-A4DD-DD265D57993A}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,7 +664,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -603,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -614,18 +697,18 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -658,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -692,48 +775,105 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
+    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>19</v>
+      <c r="A25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A18:C18"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" xr:uid="{4DD25045-89B3-43CF-87F5-CD0A06E55FFB}"/>
-    <hyperlink ref="C16" r:id="rId2" display="https://www.digikey.com/en/products/detail/mill-max-manufacturing-corp./110-44-628-41-001000/947065?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-947065_sig-Cj0KCQiAsvWrBhC0ARIsAO4E6f-n5nWNgybS2qUO86ZqxEnQ_h0rnbVowhkTPqAOPzXCz3sslOpRflsaApoTEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQiAsvWrBhC0ARIsAO4E6f-n5nWNgybS2qUO86ZqxEnQ_h0rnbVowhkTPqAOPzXCz3sslOpRflsaApoTEALw_wcB" xr:uid="{053A8A85-F9CF-4E0A-93A2-4C09F31616E8}"/>
+    <hyperlink ref="C19" r:id="rId1" xr:uid="{4DD25045-89B3-43CF-87F5-CD0A06E55FFB}"/>
+    <hyperlink ref="C20" r:id="rId2" display="https://www.digikey.com/en/products/detail/mill-max-manufacturing-corp./110-44-628-41-001000/947065?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-947065_sig-Cj0KCQiAsvWrBhC0ARIsAO4E6f-n5nWNgybS2qUO86ZqxEnQ_h0rnbVowhkTPqAOPzXCz3sslOpRflsaApoTEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQiAsvWrBhC0ARIsAO4E6f-n5nWNgybS2qUO86ZqxEnQ_h0rnbVowhkTPqAOPzXCz3sslOpRflsaApoTEALw_wcB" xr:uid="{053A8A85-F9CF-4E0A-93A2-4C09F31616E8}"/>
     <hyperlink ref="C14" r:id="rId3" xr:uid="{EF6D0EB1-CFD2-46DC-BF86-D05BC61DEFD4}"/>
     <hyperlink ref="C11" r:id="rId4" xr:uid="{8DB065A2-37D7-475A-8156-0BCC7FB349C2}"/>
     <hyperlink ref="C10" r:id="rId5" xr:uid="{B567972A-FFD1-46F9-AAE1-F5D36169BF5A}"/>
@@ -746,9 +886,13 @@
     <hyperlink ref="C5" r:id="rId12" xr:uid="{53C239B4-8FD1-43A9-96FC-F7915567B314}"/>
     <hyperlink ref="C6" r:id="rId13" display="https://www.digikey.com/en/products/detail/kemet/C322C105K5R5TA/6873900?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Medium%20ROAS%20Categories&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-20223376311_adg-_ad-__dev-c_ext-_prd-6873900_sig-Cj0KCQiAsvWrBhC0ARIsAO4E6f-hptidbDFN9jsBPWsE-qS2SHHyEruGHlnYzrtlqytt3fgkfkHBR14aAvdJEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQiAsvWrBhC0ARIsAO4E6f-hptidbDFN9jsBPWsE-qS2SHHyEruGHlnYzrtlqytt3fgkfkHBR14aAvdJEALw_wcB" xr:uid="{69E4274B-9E6E-49F2-86BD-826FB2CD2167}"/>
     <hyperlink ref="C7" r:id="rId14" display="https://www.digikey.com/en/products/detail/kemet/C322C103K5R5TA7301/6562556?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-6562556_sig-Cj0KCQiAsvWrBhC0ARIsAO4E6f99l6j3AgD_0fBeV8JLOapC1XRNzTq7SYgEgKud7fCxP74o-l6Nt5QaAvn0EALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQiAsvWrBhC0ARIsAO4E6f99l6j3AgD_0fBeV8JLOapC1XRNzTq7SYgEgKud7fCxP74o-l6Nt5QaAvn0EALw_wcB" xr:uid="{04F2AFB8-8FA7-4ACF-B836-F0D36B08019F}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{FE1853CC-7111-4509-BD2C-450850A49218}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{FE1853CC-7111-4509-BD2C-450850A49218}"/>
+    <hyperlink ref="C21" r:id="rId16" display="https://www.digikey.com/en/products/detail/on-shore-technology-inc./SA083040/3313521?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-3313521_sig-CjwKCAiAhJWsBhAaEiwAmrNyq5dclVZk8-MBYFG0oFTDynfyj3FFGwbIrs7jaRJfWEbyVEt59HuM7xoCXo8QAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAhJWsBhAaEiwAmrNyq5dclVZk8-MBYFG0oFTDynfyj3FFGwbIrs7jaRJfWEbyVEt59HuM7xoCXo8QAvD_BwE" xr:uid="{08261B2E-0044-4A9E-ADE4-2A4F9AC4745B}"/>
+    <hyperlink ref="C22" r:id="rId17" display="https://www.digikey.com/en/products/detail/on-shore-technology-inc./SA143040/3313523?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-3313523_sig-CjwKCAiAhJWsBhAaEiwAmrNyqxTndQQCCuQQPSV_d0JFNoRku27pWZsp-P1NJmj3MW2GJU_XtduBPxoC2n8QAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAhJWsBhAaEiwAmrNyqxTndQQCCuQQPSV_d0JFNoRku27pWZsp-P1NJmj3MW2GJU_XtduBPxoC2n8QAvD_BwE" xr:uid="{ACEF4F43-3989-487F-8F1A-6E19AD6E0275}"/>
+    <hyperlink ref="C26" r:id="rId18" location="description" xr:uid="{253442A3-7CDD-4330-A979-2BF52FDD6738}"/>
+    <hyperlink ref="C27" r:id="rId19" xr:uid="{CBFEA38F-3B7B-4014-8652-494F0CCC6980}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId16"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>